<commit_message>
Update assumptions in MPNVbT
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Dropbox (Energy Innovation)\Documents\EPS_Models by Region\United States\Model\InputData\trans\MPNVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\MPNVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAB689A-F61D-45D1-951B-F8A3E68C7F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="338" windowWidth="15397" windowHeight="9194" firstSheet="15" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="338" windowWidth="15398" windowHeight="9195"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +33,7 @@
     <sheet name="MPNVbT-motorbikes-psgr" sheetId="17" r:id="rId19"/>
     <sheet name="MPNVbT-motorbikes-frgt" sheetId="18" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1839,7 +1838,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -2192,16 +2191,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Body: normal cell" xfId="4"/>
     <cellStyle name="Comma" xfId="9" builtinId="3"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Footnotes: top row" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Header: bottom row" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="6"/>
+    <cellStyle name="Footnotes: top row" xfId="2"/>
+    <cellStyle name="Header: bottom row" xfId="5"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Parent row" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Table title" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Parent row" xfId="3"/>
+    <cellStyle name="Table title" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2292,23 +2291,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2344,23 +2326,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2536,10 +2501,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -3040,7 +3005,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B14" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -3048,7 +3013,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -4196,7 +4161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -5344,7 +5309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -6494,7 +6459,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -7642,7 +7607,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -8790,14 +8755,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2:AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8953,139 +8918,139 @@
       </c>
       <c r="B2" s="16">
         <f>Data!I50</f>
-        <v>0.5118281341400337</v>
+        <v>0.75216927859794647</v>
       </c>
       <c r="C2" s="16">
         <f>Data!J50</f>
-        <v>0.51444491476645848</v>
+        <v>0.75379348625303</v>
       </c>
       <c r="D2" s="16">
         <f>Data!K50</f>
-        <v>0.51534689283469481</v>
+        <v>0.75435333436117979</v>
       </c>
       <c r="E2" s="16">
         <f>Data!L50</f>
-        <v>0.51655353677595117</v>
+        <v>0.75510228530745249</v>
       </c>
       <c r="F2" s="16">
         <f>Data!M50</f>
-        <v>0.51816278972650143</v>
+        <v>0.75610113134554036</v>
       </c>
       <c r="G2" s="16">
         <f>Data!N50</f>
-        <v>0.52030019065995547</v>
+        <v>0.75742779316924924</v>
       </c>
       <c r="H2" s="16">
         <f>Data!O50</f>
-        <v>0.52312364284477286</v>
+        <v>0.75918027964290846</v>
       </c>
       <c r="I2" s="16">
         <f>Data!P50</f>
-        <v>0.52682661585159252</v>
+        <v>0.76147867525296065</v>
       </c>
       <c r="J2" s="16">
         <f>Data!Q50</f>
-        <v>0.53163753045259587</v>
+        <v>0.7644647583215971</v>
       </c>
       <c r="K2" s="16">
         <f>Data!R50</f>
-        <v>0.53781192760358398</v>
+        <v>0.76829714037796482</v>
       </c>
       <c r="L2" s="16">
         <f>Data!S50</f>
-        <v>0.54561306694160605</v>
+        <v>0.77313922385383504</v>
       </c>
       <c r="M2" s="16">
         <f>Data!T50</f>
-        <v>0.55527676152547534</v>
+        <v>0.77913737538438765</v>
       </c>
       <c r="N2" s="16">
         <f>Data!U50</f>
-        <v>0.56695901835441231</v>
+        <v>0.78638842683998322</v>
       </c>
       <c r="O2" s="16">
         <f>Data!V50</f>
-        <v>0.58067183042758774</v>
+        <v>0.79489982214651456</v>
       </c>
       <c r="P2" s="16">
         <f>Data!W50</f>
-        <v>0.59622283284194855</v>
+        <v>0.80455216247285544</v>
       </c>
       <c r="Q2" s="16">
         <f>Data!X50</f>
-        <v>0.61318395394167213</v>
+        <v>0.81507974833572117</v>
       </c>
       <c r="R2" s="16">
         <f>Data!Y50</f>
-        <v>0.63091406707001685</v>
+        <v>0.82608463929897324</v>
       </c>
       <c r="S2" s="16">
         <f>Data!Z50</f>
-        <v>0.64864418019836156</v>
+        <v>0.83708953026222532</v>
       </c>
       <c r="T2" s="16">
         <f>Data!AA50</f>
-        <v>0.66560530129808515</v>
+        <v>0.84761711612509105</v>
       </c>
       <c r="U2" s="16">
         <f>Data!AB50</f>
-        <v>0.68115630371244595</v>
+        <v>0.85726945645143193</v>
       </c>
       <c r="V2" s="16">
         <f>Data!AC50</f>
-        <v>0.69486911578562138</v>
+        <v>0.86578085175796327</v>
       </c>
       <c r="W2" s="16">
         <f>Data!AD50</f>
-        <v>0.70655137261455836</v>
+        <v>0.87303190321355884</v>
       </c>
       <c r="X2" s="16">
         <f>Data!AE50</f>
-        <v>0.71621506719842765</v>
+        <v>0.87903005474411144</v>
       </c>
       <c r="Y2" s="16">
         <f>Data!AF50</f>
-        <v>0.72401620653644971</v>
+        <v>0.88387213821998167</v>
       </c>
       <c r="Z2" s="16">
         <f>Data!AG50</f>
-        <v>0.73019060368743782</v>
+        <v>0.88770452027634938</v>
       </c>
       <c r="AA2" s="16">
         <f>Data!AH50</f>
-        <v>0.73500151828844118</v>
+        <v>0.89069060334498584</v>
       </c>
       <c r="AB2" s="16">
         <f>Data!AI50</f>
-        <v>0.73870449129526083</v>
+        <v>0.89298899895503803</v>
       </c>
       <c r="AC2" s="16">
         <f>Data!AJ50</f>
-        <v>0.74152794348007822</v>
+        <v>0.89474148542869725</v>
       </c>
       <c r="AD2" s="16">
         <f>Data!AK50</f>
-        <v>0.74366534441353227</v>
+        <v>0.89606814725240613</v>
       </c>
       <c r="AE2" s="16">
         <f>Data!AL50</f>
-        <v>0.74527459736408264</v>
+        <v>0.897066993290494</v>
       </c>
       <c r="AF2" s="16">
         <f>Data!AM50</f>
-        <v>0.74648124130533888</v>
+        <v>0.89781594423676669</v>
       </c>
       <c r="AG2" s="16">
         <f>Data!AN50</f>
-        <v>0.74738321937357521</v>
+        <v>0.89837579234491649</v>
       </c>
       <c r="AH2" s="16">
         <f>Data!AO50</f>
-        <v>0.74805590519823717</v>
+        <v>0.89879332121793287</v>
       </c>
       <c r="AI2" s="16">
         <f>Data!AP50</f>
-        <v>0.74855672577200838</v>
+        <v>0.89910417517394592</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.45">
@@ -9376,139 +9341,139 @@
       </c>
       <c r="B5" s="16">
         <f>Data!I53</f>
-        <v>0.48817186585996641</v>
+        <v>0.24783072140205353</v>
       </c>
       <c r="C5" s="16">
         <f>Data!J53</f>
-        <v>0.49661793470319182</v>
+        <v>0.24306198845360072</v>
       </c>
       <c r="D5" s="16">
         <f>Data!K53</f>
-        <v>0.50506400354641912</v>
+        <v>0.23829325550514646</v>
       </c>
       <c r="E5" s="16">
         <f>Data!L53</f>
-        <v>0.51351007238964641</v>
+        <v>0.23352452255669398</v>
       </c>
       <c r="F5" s="16">
         <f>Data!M53</f>
-        <v>0.5219561412328737</v>
+        <v>0.22875578960823972</v>
       </c>
       <c r="G5" s="16">
         <f>Data!N53</f>
-        <v>0.530402210076101</v>
+        <v>0.22398705665978724</v>
       </c>
       <c r="H5" s="16">
         <f>Data!O53</f>
-        <v>0.53884827891932829</v>
+        <v>0.21921832371133299</v>
       </c>
       <c r="I5" s="16">
         <f>Data!P53</f>
-        <v>0.54729434776255559</v>
+        <v>0.2144495907628805</v>
       </c>
       <c r="J5" s="16">
         <f>Data!Q53</f>
-        <v>0.55574041660577933</v>
+        <v>0.20968085781442625</v>
       </c>
       <c r="K5" s="16">
         <f>Data!R53</f>
-        <v>0.56418648544900663</v>
+        <v>0.20491212486597377</v>
       </c>
       <c r="L5" s="16">
         <f>Data!S53</f>
-        <v>0.57263255429223392</v>
+        <v>0.20014339191751951</v>
       </c>
       <c r="M5" s="16">
         <f>Data!T53</f>
-        <v>0.58107862313546121</v>
+        <v>0.19537465896906703</v>
       </c>
       <c r="N5" s="16">
         <f>Data!U53</f>
-        <v>0.58952469197868851</v>
+        <v>0.19060592602061277</v>
       </c>
       <c r="O5" s="16">
         <f>Data!V53</f>
-        <v>0.5979707608219158</v>
+        <v>0.18583719307216029</v>
       </c>
       <c r="P5" s="16">
         <f>Data!W53</f>
-        <v>0.6064168296651431</v>
+        <v>0.18106846012370603</v>
       </c>
       <c r="Q5" s="16">
         <f>Data!X53</f>
-        <v>0.61486289850837039</v>
+        <v>0.17629972717525355</v>
       </c>
       <c r="R5" s="16">
         <f>Data!Y53</f>
-        <v>0.62330896735159413</v>
+        <v>0.17153099422679929</v>
       </c>
       <c r="S5" s="16">
         <f>Data!Z53</f>
-        <v>0.63175503619482143</v>
+        <v>0.16676226127834681</v>
       </c>
       <c r="T5" s="16">
         <f>Data!AA53</f>
-        <v>0.64020110503804872</v>
+        <v>0.16199352832989256</v>
       </c>
       <c r="U5" s="16">
         <f>Data!AB53</f>
-        <v>0.64864717388127602</v>
+        <v>0.15722479538144007</v>
       </c>
       <c r="V5" s="16">
         <f>Data!AC53</f>
-        <v>0.65709324272450331</v>
+        <v>0.15245606243298582</v>
       </c>
       <c r="W5" s="16">
         <f>Data!AD53</f>
-        <v>0.66553931156773061</v>
+        <v>0.14768732948453334</v>
       </c>
       <c r="X5" s="16">
         <f>Data!AE53</f>
-        <v>0.6739853804109579</v>
+        <v>0.14291859653607908</v>
       </c>
       <c r="Y5" s="16">
         <f>Data!AF53</f>
-        <v>0.6824314492541852</v>
+        <v>0.1381498635876266</v>
       </c>
       <c r="Z5" s="16">
         <f>Data!AG53</f>
-        <v>0.69087751809741249</v>
+        <v>0.13338113063917234</v>
       </c>
       <c r="AA5" s="16">
         <f>Data!AH53</f>
-        <v>0.69932358694063623</v>
+        <v>0.12861239769071986</v>
       </c>
       <c r="AB5" s="16">
         <f>Data!AI53</f>
-        <v>0.70776965578386353</v>
+        <v>0.1238436647422656</v>
       </c>
       <c r="AC5" s="16">
         <f>Data!AJ53</f>
-        <v>0.71621572462709082</v>
+        <v>0.11907493179381312</v>
       </c>
       <c r="AD5" s="16">
         <f>Data!AK53</f>
-        <v>0.72466179347031812</v>
+        <v>0.11430619884535886</v>
       </c>
       <c r="AE5" s="16">
         <f>Data!AL53</f>
-        <v>0.73310786231354541</v>
+        <v>0.10953746589690638</v>
       </c>
       <c r="AF5" s="16">
         <f>Data!AM53</f>
-        <v>0.74155393115677271</v>
+        <v>0.1047687329484539</v>
       </c>
       <c r="AG5" s="16">
         <f>Data!AN53</f>
-        <v>0.75</v>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="AH5" s="16">
         <f>Data!AO53</f>
-        <v>0.75844606884322729</v>
+        <v>9.5231267051547164E-2</v>
       </c>
       <c r="AI5" s="16">
         <f>Data!AP53</f>
-        <v>0.76689213768645459</v>
+        <v>9.0462534103092906E-2</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.45">
@@ -9940,13 +9905,13 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="AH1" sqref="AH1:AI8"/>
     </sheetView>
   </sheetViews>
@@ -11026,7 +10991,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -12112,7 +12077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -13198,7 +13163,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -14284,7 +14249,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20691,7 +20656,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -21777,7 +21742,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26439,7 +26404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI281"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -49971,10 +49936,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:H5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -50099,7 +50066,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="6">
-        <v>1258.1247365296165</v>
+        <v>1861.3933137463398</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -50108,7 +50075,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="5">
-        <v>1199.9752634703832</v>
+        <v>613.30668625366241</v>
       </c>
       <c r="F5" s="6">
         <v>0</v>
@@ -50191,7 +50158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -50408,11 +50375,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -50532,7 +50499,7 @@
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="24">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
@@ -50617,14 +50584,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:AP91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -57351,11 +57318,11 @@
       </c>
       <c r="D50" s="31">
         <f>'SYVbT-passenger'!B5/SUM('SYVbT-passenger'!B5:H5)</f>
-        <v>0.5118281341400337</v>
+        <v>0.75216927859794647</v>
       </c>
       <c r="E50" s="16">
         <f>Assumptions!A28</f>
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="F50" s="9" t="str">
         <f t="shared" si="1"/>
@@ -57364,139 +57331,139 @@
       <c r="H50" s="32"/>
       <c r="I50" s="31">
         <f t="shared" si="5"/>
-        <v>0.5118281341400337</v>
+        <v>0.75216927859794647</v>
       </c>
       <c r="J50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,J$7))</f>
-        <v>0.51444491476645848</v>
+        <v>0.75379348625303</v>
       </c>
       <c r="K50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,K$7))</f>
-        <v>0.51534689283469481</v>
+        <v>0.75435333436117979</v>
       </c>
       <c r="L50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,L$7))</f>
-        <v>0.51655353677595117</v>
+        <v>0.75510228530745249</v>
       </c>
       <c r="M50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,M$7))</f>
-        <v>0.51816278972650143</v>
+        <v>0.75610113134554036</v>
       </c>
       <c r="N50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,N$7))</f>
-        <v>0.52030019065995547</v>
+        <v>0.75742779316924924</v>
       </c>
       <c r="O50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,O$7))</f>
-        <v>0.52312364284477286</v>
+        <v>0.75918027964290846</v>
       </c>
       <c r="P50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,P$7))</f>
-        <v>0.52682661585159252</v>
+        <v>0.76147867525296065</v>
       </c>
       <c r="Q50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,Q$7))</f>
-        <v>0.53163753045259587</v>
+        <v>0.7644647583215971</v>
       </c>
       <c r="R50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,R$7))</f>
-        <v>0.53781192760358398</v>
+        <v>0.76829714037796482</v>
       </c>
       <c r="S50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,S$7))</f>
-        <v>0.54561306694160605</v>
+        <v>0.77313922385383504</v>
       </c>
       <c r="T50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,T$7))</f>
-        <v>0.55527676152547534</v>
+        <v>0.77913737538438765</v>
       </c>
       <c r="U50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,U$7))</f>
-        <v>0.56695901835441231</v>
+        <v>0.78638842683998322</v>
       </c>
       <c r="V50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,V$7))</f>
-        <v>0.58067183042758774</v>
+        <v>0.79489982214651456</v>
       </c>
       <c r="W50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,W$7))</f>
-        <v>0.59622283284194855</v>
+        <v>0.80455216247285544</v>
       </c>
       <c r="X50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,X$7))</f>
-        <v>0.61318395394167213</v>
+        <v>0.81507974833572117</v>
       </c>
       <c r="Y50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,Y$7))</f>
-        <v>0.63091406707001685</v>
+        <v>0.82608463929897324</v>
       </c>
       <c r="Z50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,Z$7))</f>
-        <v>0.64864418019836156</v>
+        <v>0.83708953026222532</v>
       </c>
       <c r="AA50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AA$7))</f>
-        <v>0.66560530129808515</v>
+        <v>0.84761711612509105</v>
       </c>
       <c r="AB50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AB$7))</f>
-        <v>0.68115630371244595</v>
+        <v>0.85726945645143193</v>
       </c>
       <c r="AC50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AC$7))</f>
-        <v>0.69486911578562138</v>
+        <v>0.86578085175796327</v>
       </c>
       <c r="AD50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AD$7))</f>
-        <v>0.70655137261455836</v>
+        <v>0.87303190321355884</v>
       </c>
       <c r="AE50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AE$7))</f>
-        <v>0.71621506719842765</v>
+        <v>0.87903005474411144</v>
       </c>
       <c r="AF50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AF$7))</f>
-        <v>0.72401620653644971</v>
+        <v>0.88387213821998167</v>
       </c>
       <c r="AG50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AG$7))</f>
-        <v>0.73019060368743782</v>
+        <v>0.88770452027634938</v>
       </c>
       <c r="AH50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AH$7))</f>
-        <v>0.73500151828844118</v>
+        <v>0.89069060334498584</v>
       </c>
       <c r="AI50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AI$7))</f>
-        <v>0.73870449129526083</v>
+        <v>0.89298899895503803</v>
       </c>
       <c r="AJ50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AJ$7))</f>
-        <v>0.74152794348007822</v>
+        <v>0.89474148542869725</v>
       </c>
       <c r="AK50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AK$7))</f>
-        <v>0.74366534441353227</v>
+        <v>0.89606814725240613</v>
       </c>
       <c r="AL50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AL$7))</f>
-        <v>0.74527459736408264</v>
+        <v>0.897066993290494</v>
       </c>
       <c r="AM50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AM$7))</f>
-        <v>0.74648124130533888</v>
+        <v>0.89781594423676669</v>
       </c>
       <c r="AN50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AN$7))</f>
-        <v>0.74738321937357521</v>
+        <v>0.89837579234491649</v>
       </c>
       <c r="AO50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AO$7))</f>
-        <v>0.74805590519823717</v>
+        <v>0.89879332121793287</v>
       </c>
       <c r="AP50" s="16">
         <f>IF($F50="s-curve",$D50+($E50-$D50)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D50:$E50,$D$7:$E$7,AP$7))</f>
-        <v>0.74855672577200838</v>
+        <v>0.89910417517394592</v>
       </c>
     </row>
     <row r="51" spans="1:42" x14ac:dyDescent="0.45">
@@ -57808,12 +57775,12 @@
         <v>5</v>
       </c>
       <c r="D53" s="31">
-        <f>'SYVbT-passenger'!E5/SUM('SYVbT-passenger'!B5:H5)</f>
-        <v>0.48817186585996641</v>
+        <f>1-D50</f>
+        <v>0.24783072140205353</v>
       </c>
       <c r="E53" s="16">
-        <f>Assumptions!A28</f>
-        <v>0.75</v>
+        <f>1-E50</f>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="F53" s="9" t="str">
         <f t="shared" si="1"/>
@@ -57822,139 +57789,139 @@
       <c r="H53" s="32"/>
       <c r="I53" s="31">
         <f t="shared" si="5"/>
-        <v>0.48817186585996641</v>
+        <v>0.24783072140205353</v>
       </c>
       <c r="J53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:J$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,J$7))</f>
-        <v>0.49661793470319182</v>
+        <v>0.24306198845360072</v>
       </c>
       <c r="K53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:K$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,K$7))</f>
-        <v>0.50506400354641912</v>
+        <v>0.23829325550514646</v>
       </c>
       <c r="L53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:L$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,L$7))</f>
-        <v>0.51351007238964641</v>
+        <v>0.23352452255669398</v>
       </c>
       <c r="M53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:M$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,M$7))</f>
-        <v>0.5219561412328737</v>
+        <v>0.22875578960823972</v>
       </c>
       <c r="N53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:N$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,N$7))</f>
-        <v>0.530402210076101</v>
+        <v>0.22398705665978724</v>
       </c>
       <c r="O53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:O$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,O$7))</f>
-        <v>0.53884827891932829</v>
+        <v>0.21921832371133299</v>
       </c>
       <c r="P53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:P$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,P$7))</f>
-        <v>0.54729434776255559</v>
+        <v>0.2144495907628805</v>
       </c>
       <c r="Q53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:Q$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,Q$7))</f>
-        <v>0.55574041660577933</v>
+        <v>0.20968085781442625</v>
       </c>
       <c r="R53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:R$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,R$7))</f>
-        <v>0.56418648544900663</v>
+        <v>0.20491212486597377</v>
       </c>
       <c r="S53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:S$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,S$7))</f>
-        <v>0.57263255429223392</v>
+        <v>0.20014339191751951</v>
       </c>
       <c r="T53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:T$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,T$7))</f>
-        <v>0.58107862313546121</v>
+        <v>0.19537465896906703</v>
       </c>
       <c r="U53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:U$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,U$7))</f>
-        <v>0.58952469197868851</v>
+        <v>0.19060592602061277</v>
       </c>
       <c r="V53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:V$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,V$7))</f>
-        <v>0.5979707608219158</v>
+        <v>0.18583719307216029</v>
       </c>
       <c r="W53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:W$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,W$7))</f>
-        <v>0.6064168296651431</v>
+        <v>0.18106846012370603</v>
       </c>
       <c r="X53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:X$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,X$7))</f>
-        <v>0.61486289850837039</v>
+        <v>0.17629972717525355</v>
       </c>
       <c r="Y53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:Y$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,Y$7))</f>
-        <v>0.62330896735159413</v>
+        <v>0.17153099422679929</v>
       </c>
       <c r="Z53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:Z$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,Z$7))</f>
-        <v>0.63175503619482143</v>
+        <v>0.16676226127834681</v>
       </c>
       <c r="AA53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AA$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AA$7))</f>
-        <v>0.64020110503804872</v>
+        <v>0.16199352832989256</v>
       </c>
       <c r="AB53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AB$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AB$7))</f>
-        <v>0.64864717388127602</v>
+        <v>0.15722479538144007</v>
       </c>
       <c r="AC53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AC$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AC$7))</f>
-        <v>0.65709324272450331</v>
+        <v>0.15245606243298582</v>
       </c>
       <c r="AD53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AD$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AD$7))</f>
-        <v>0.66553931156773061</v>
+        <v>0.14768732948453334</v>
       </c>
       <c r="AE53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AE$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AE$7))</f>
-        <v>0.6739853804109579</v>
+        <v>0.14291859653607908</v>
       </c>
       <c r="AF53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AF$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AF$7))</f>
-        <v>0.6824314492541852</v>
+        <v>0.1381498635876266</v>
       </c>
       <c r="AG53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AG$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AG$7))</f>
-        <v>0.69087751809741249</v>
+        <v>0.13338113063917234</v>
       </c>
       <c r="AH53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AH$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AH$7))</f>
-        <v>0.69932358694063623</v>
+        <v>0.12861239769071986</v>
       </c>
       <c r="AI53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AI$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AI$7))</f>
-        <v>0.70776965578386353</v>
+        <v>0.1238436647422656</v>
       </c>
       <c r="AJ53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AJ$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AJ$7))</f>
-        <v>0.71621572462709082</v>
+        <v>0.11907493179381312</v>
       </c>
       <c r="AK53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AK$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AK$7))</f>
-        <v>0.72466179347031812</v>
+        <v>0.11430619884535886</v>
       </c>
       <c r="AL53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AL$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AL$7))</f>
-        <v>0.73310786231354541</v>
+        <v>0.10953746589690638</v>
       </c>
       <c r="AM53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AM$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AM$7))</f>
-        <v>0.74155393115677271</v>
+        <v>0.1047687329484539</v>
       </c>
       <c r="AN53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AN$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AN$7))</f>
-        <v>0.75</v>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="AO53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AO$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AO$7))</f>
-        <v>0.75844606884322729</v>
+        <v>9.5231267051547164E-2</v>
       </c>
       <c r="AP53" s="16">
         <f>IF($F53="s-curve",$D53+($E53-$D53)*$I$2/(1+EXP($I$3*(COUNT($I$7:AP$7)+$I$4))),TREND($D53:$E53,$D$7:$E$7,AP$7))</f>
-        <v>0.76689213768645459</v>
+        <v>9.0462534103092906E-2</v>
       </c>
     </row>
     <row r="54" spans="1:42" x14ac:dyDescent="0.45">
@@ -63793,7 +63760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>

</xml_diff>

<commit_message>
Recalibrate MPNVbT for EV sales
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\trans\MPNVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\trans\MPNVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="338" windowWidth="15398" windowHeight="9195"/>
+    <workbookView xWindow="2520" yWindow="338" windowWidth="15398" windowHeight="9195" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <sheet name="MPNVbT-motorbikes-psgr" sheetId="17" r:id="rId19"/>
     <sheet name="MPNVbT-motorbikes-frgt" sheetId="18" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1839,12 +1839,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -2102,7 +2103,7 @@
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2208,6 +2209,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2">
       <alignment wrapText="1"/>
     </xf>
@@ -2236,6 +2238,903 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$10:$AN$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0" formatCode="0.0000">
+                  <c:v>3.0819144090348839E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0148104092397455E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4653792463561118E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.1277042374426013E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0944668273484187E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.4911802772556088E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.4793989967857678E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.12250774967825262</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16002738639012218</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.20886544924044625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26928483805044562</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.33950091317215791</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.41540957204517448</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.49131823091819105</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.56153430603990329</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.62195369484990271</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.6707917577002267</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.70831139441209623</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.73602515412249125</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.7559073413177928</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.76987447581686475</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.77954210171592286</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.78616535162678769</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.79067103999795141</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.7937215065339891</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.79578004391674451</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.79716615320077544</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.79809810560403771</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.79872408196536759</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.79914425858201432</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.79942616890305629</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.79961525488432961</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7845-4F26-8099-2F927049CEFA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="343204120"/>
+        <c:axId val="343203464"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="343204120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="343203464"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="343203464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="343204120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2282,6 +3181,41 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>597693</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>226217</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>602456</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>69055</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2576,7 +3510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
@@ -3225,131 +4159,131 @@
       </c>
       <c r="B2" s="16">
         <f>Data!I17</f>
-        <v>3.9166926468788582E-2</v>
+        <v>3.0819144090348839E-2</v>
       </c>
       <c r="C2" s="16">
         <f>Data!J17</f>
-        <v>5.3362304749083656E-2</v>
+        <v>4.2183046433416922E-2</v>
       </c>
       <c r="D2" s="16">
         <f>Data!K17</f>
-        <v>5.8230148407061193E-2</v>
+        <v>4.6079927436395739E-2</v>
       </c>
       <c r="E2" s="16">
         <f>Data!L17</f>
-        <v>6.4722197553938501E-2</v>
+        <v>5.1277042374426027E-2</v>
       </c>
       <c r="F2" s="16">
         <f>Data!M17</f>
-        <v>7.3344901586776062E-2</v>
+        <v>5.8179821900799344E-2</v>
       </c>
       <c r="G2" s="16">
         <f>Data!N17</f>
-        <v>8.4735273958891508E-2</v>
+        <v>6.7298217813332228E-2</v>
       </c>
       <c r="H2" s="16">
         <f>Data!O17</f>
-        <v>9.9673809719607862E-2</v>
+        <v>7.9257044001772636E-2</v>
       </c>
       <c r="I2" s="16">
         <f>Data!P17</f>
-        <v>0.11908200407492263</v>
+        <v>9.4793989967857706E-2</v>
       </c>
       <c r="J2" s="16">
         <f>Data!Q17</f>
-        <v>0.14399076049065435</v>
+        <v>0.11473433039461256</v>
       </c>
       <c r="K2" s="16">
         <f>Data!R17</f>
-        <v>0.17546212114079962</v>
+        <v>0.13992826760220153</v>
       </c>
       <c r="L2" s="16">
         <f>Data!S17</f>
-        <v>0.21444740319819114</v>
+        <v>0.17113736463148846</v>
       </c>
       <c r="M2" s="16">
         <f>Data!T17</f>
-        <v>0.26157597018573009</v>
+        <v>0.20886544924044628</v>
       </c>
       <c r="N2" s="16">
         <f>Data!U17</f>
-        <v>0.31689620426733145</v>
+        <v>0.25315125306235869</v>
       </c>
       <c r="O2" s="16">
         <f>Data!V17</f>
-        <v>0.37963206684425987</v>
+        <v>0.30337352975377885</v>
       </c>
       <c r="P2" s="16">
         <f>Data!W17</f>
-        <v>0.44805663100484905</v>
+        <v>0.35814981324791401</v>
       </c>
       <c r="Q2" s="16">
         <f>Data!X17</f>
-        <v>0.5195834632343943</v>
+        <v>0.41540957204517448</v>
       </c>
       <c r="R2" s="16">
         <f>Data!Y17</f>
-        <v>0.59111029546393956</v>
+        <v>0.47266933084243495</v>
       </c>
       <c r="S2" s="16">
         <f>Data!Z17</f>
-        <v>0.65953485962452862</v>
+        <v>0.52744561433657</v>
       </c>
       <c r="T2" s="16">
         <f>Data!AA17</f>
-        <v>0.72227072220145716</v>
+        <v>0.5776678910279901</v>
       </c>
       <c r="U2" s="16">
         <f>Data!AB17</f>
-        <v>0.77759095628305852</v>
+        <v>0.62195369484990259</v>
       </c>
       <c r="V2" s="16">
         <f>Data!AC17</f>
-        <v>0.82471952327059739</v>
+        <v>0.65968177945886042</v>
       </c>
       <c r="W2" s="16">
         <f>Data!AD17</f>
-        <v>0.86370480532798899</v>
+        <v>0.6908908764881474</v>
       </c>
       <c r="X2" s="16">
         <f>Data!AE17</f>
-        <v>0.89517616597813421</v>
+        <v>0.71608481369573629</v>
       </c>
       <c r="Y2" s="16">
         <f>Data!AF17</f>
-        <v>0.92008492239386597</v>
+        <v>0.73602515412249125</v>
       </c>
       <c r="Z2" s="16">
         <f>Data!AG17</f>
-        <v>0.93949311674918079</v>
+        <v>0.75156210008857627</v>
       </c>
       <c r="AA2" s="16">
         <f>Data!AH17</f>
-        <v>0.95443165250989714</v>
+        <v>0.76352092627701673</v>
       </c>
       <c r="AB2" s="16">
         <f>Data!AI17</f>
-        <v>0.96582202488201252</v>
+        <v>0.77263932218954956</v>
       </c>
       <c r="AC2" s="16">
         <f>Data!AJ17</f>
-        <v>0.97444472891485001</v>
+        <v>0.77954210171592286</v>
       </c>
       <c r="AD2" s="16">
         <f>Data!AK17</f>
-        <v>0.98093677806172741</v>
+        <v>0.78473921665395319</v>
       </c>
       <c r="AE2" s="16">
         <f>Data!AL17</f>
-        <v>0.98580462171970495</v>
+        <v>0.78863609765693199</v>
       </c>
       <c r="AF2" s="16">
         <f>Data!AM17</f>
-        <v>0.98944338214353611</v>
+        <v>0.79154905406357012</v>
       </c>
       <c r="AG2" s="16">
         <f>Data!AN17</f>
-        <v>0.99215713167099218</v>
+        <v>0.7937215065339891</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">
@@ -4315,127 +5249,127 @@
       </c>
       <c r="C2" s="16">
         <f>Data!J24</f>
-        <v>1.5070634542928764E-2</v>
+        <v>1.2115828204274155E-2</v>
       </c>
       <c r="D2" s="16">
         <f>Data!K24</f>
-        <v>2.01353833789924E-2</v>
+        <v>1.6167322232176901E-2</v>
       </c>
       <c r="E2" s="16">
         <f>Data!L24</f>
-        <v>2.6890037116983612E-2</v>
+        <v>2.1570638401610439E-2</v>
       </c>
       <c r="F2" s="16">
         <f>Data!M24</f>
-        <v>3.5861531125930435E-2</v>
+        <v>2.8747293271403202E-2</v>
       </c>
       <c r="G2" s="16">
         <f>Data!N24</f>
-        <v>4.7712646171390136E-2</v>
+        <v>3.8227471535876779E-2</v>
       </c>
       <c r="H2" s="16">
         <f>Data!O24</f>
-        <v>6.3255448472074108E-2</v>
+        <v>5.0660777260674819E-2</v>
       </c>
       <c r="I2" s="16">
         <f>Data!P24</f>
-        <v>8.3448707885836276E-2</v>
+        <v>6.6814168587051803E-2</v>
       </c>
       <c r="J2" s="16">
         <f>Data!Q24</f>
-        <v>0.10936502811473713</v>
+        <v>8.7545663875614535E-2</v>
       </c>
       <c r="K2" s="16">
         <f>Data!R24</f>
-        <v>0.14210941113553172</v>
+        <v>0.11373919815543415</v>
       </c>
       <c r="L2" s="16">
         <f>Data!S24</f>
-        <v>0.18267165507699426</v>
+        <v>0.146186550315723</v>
       </c>
       <c r="M2" s="16">
         <f>Data!T24</f>
-        <v>0.23170658133316255</v>
+        <v>0.18541153803296609</v>
       </c>
       <c r="N2" s="16">
         <f>Data!U24</f>
-        <v>0.28926452913544826</v>
+        <v>0.23145442966044902</v>
       </c>
       <c r="O2" s="16">
         <f>Data!V24</f>
-        <v>0.3545380689799798</v>
+        <v>0.2836693302251389</v>
       </c>
       <c r="P2" s="16">
         <f>Data!W24</f>
-        <v>0.42573041944147549</v>
+        <v>0.34061892280380729</v>
       </c>
       <c r="Q2" s="16">
         <f>Data!X24</f>
-        <v>0.5001505252902364</v>
+        <v>0.40015052529023648</v>
       </c>
       <c r="R2" s="16">
         <f>Data!Y24</f>
-        <v>0.57457063113899742</v>
+        <v>0.45968212777666567</v>
       </c>
       <c r="S2" s="16">
         <f>Data!Z24</f>
-        <v>0.64576298160049306</v>
+        <v>0.516631720355334</v>
       </c>
       <c r="T2" s="16">
         <f>Data!AA24</f>
-        <v>0.71103652144502461</v>
+        <v>0.56884662092002392</v>
       </c>
       <c r="U2" s="16">
         <f>Data!AB24</f>
-        <v>0.76859446924731034</v>
+        <v>0.61488951254750679</v>
       </c>
       <c r="V2" s="16">
         <f>Data!AC24</f>
-        <v>0.81762939550347857</v>
+        <v>0.65411450026474993</v>
       </c>
       <c r="W2" s="16">
         <f>Data!AD24</f>
-        <v>0.85819163944494126</v>
+        <v>0.68656185242503887</v>
       </c>
       <c r="X2" s="16">
         <f>Data!AE24</f>
-        <v>0.89093602246573578</v>
+        <v>0.71275538670485838</v>
       </c>
       <c r="Y2" s="16">
         <f>Data!AF24</f>
-        <v>0.91685234269463667</v>
+        <v>0.73348688199342116</v>
       </c>
       <c r="Z2" s="16">
         <f>Data!AG24</f>
-        <v>0.93704560210839882</v>
+        <v>0.74964027331979821</v>
       </c>
       <c r="AA2" s="16">
         <f>Data!AH24</f>
-        <v>0.95258840440908288</v>
+        <v>0.76207357904459627</v>
       </c>
       <c r="AB2" s="16">
         <f>Data!AI24</f>
-        <v>0.96443951945454254</v>
+        <v>0.77155375730906972</v>
       </c>
       <c r="AC2" s="16">
         <f>Data!AJ24</f>
-        <v>0.97341101346348924</v>
+        <v>0.77873041217886241</v>
       </c>
       <c r="AD2" s="16">
         <f>Data!AK24</f>
-        <v>0.98016566720148057</v>
+        <v>0.78413372834829609</v>
       </c>
       <c r="AE2" s="16">
         <f>Data!AL24</f>
-        <v>0.98523041603754413</v>
+        <v>0.78818522237619881</v>
       </c>
       <c r="AF2" s="16">
         <f>Data!AM24</f>
-        <v>0.98901636499486345</v>
+        <v>0.79121375352098211</v>
       </c>
       <c r="AG2" s="16">
         <f>Data!AN24</f>
-        <v>0.99183988619362395</v>
+        <v>0.79347240042425593</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">
@@ -13933,8 +14867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI99"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81:J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -19926,7 +20860,40 @@
         <v>2.287E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="81" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C81">
+        <f>C75/C80</f>
+        <v>1.8447488281938765E-2</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ref="D81:J81" si="0">D75/D80</f>
+        <v>2.3367988763240231E-2</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="0"/>
+        <v>3.0819144090348839E-2</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="0"/>
+        <v>3.169118913337516E-2</v>
+      </c>
+      <c r="G81">
+        <f t="shared" si="0"/>
+        <v>3.2913957955998024E-2</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="0"/>
+        <v>3.5857635736925242E-2</v>
+      </c>
+      <c r="I81">
+        <f t="shared" si="0"/>
+        <v>3.9166926468788582E-2</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="0"/>
+        <v>4.0260003508194267E-2</v>
+      </c>
+    </row>
     <row r="82" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="14" t="s">
         <v>524</v>
@@ -20251,42 +21218,42 @@
     </row>
     <row r="86" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="87" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B87" s="61" t="s">
+      <c r="B87" s="62" t="s">
         <v>530</v>
       </c>
-      <c r="C87" s="61"/>
-      <c r="D87" s="61"/>
-      <c r="E87" s="61"/>
-      <c r="F87" s="61"/>
-      <c r="G87" s="61"/>
-      <c r="H87" s="61"/>
-      <c r="I87" s="61"/>
-      <c r="J87" s="61"/>
-      <c r="K87" s="61"/>
-      <c r="L87" s="61"/>
-      <c r="M87" s="61"/>
-      <c r="N87" s="61"/>
-      <c r="O87" s="61"/>
-      <c r="P87" s="61"/>
-      <c r="Q87" s="61"/>
-      <c r="R87" s="61"/>
-      <c r="S87" s="61"/>
-      <c r="T87" s="61"/>
-      <c r="U87" s="61"/>
-      <c r="V87" s="61"/>
-      <c r="W87" s="61"/>
-      <c r="X87" s="61"/>
-      <c r="Y87" s="61"/>
-      <c r="Z87" s="61"/>
-      <c r="AA87" s="61"/>
-      <c r="AB87" s="61"/>
-      <c r="AC87" s="61"/>
-      <c r="AD87" s="61"/>
-      <c r="AE87" s="61"/>
-      <c r="AF87" s="61"/>
-      <c r="AG87" s="61"/>
-      <c r="AH87" s="61"/>
-      <c r="AI87" s="61"/>
+      <c r="C87" s="62"/>
+      <c r="D87" s="62"/>
+      <c r="E87" s="62"/>
+      <c r="F87" s="62"/>
+      <c r="G87" s="62"/>
+      <c r="H87" s="62"/>
+      <c r="I87" s="62"/>
+      <c r="J87" s="62"/>
+      <c r="K87" s="62"/>
+      <c r="L87" s="62"/>
+      <c r="M87" s="62"/>
+      <c r="N87" s="62"/>
+      <c r="O87" s="62"/>
+      <c r="P87" s="62"/>
+      <c r="Q87" s="62"/>
+      <c r="R87" s="62"/>
+      <c r="S87" s="62"/>
+      <c r="T87" s="62"/>
+      <c r="U87" s="62"/>
+      <c r="V87" s="62"/>
+      <c r="W87" s="62"/>
+      <c r="X87" s="62"/>
+      <c r="Y87" s="62"/>
+      <c r="Z87" s="62"/>
+      <c r="AA87" s="62"/>
+      <c r="AB87" s="62"/>
+      <c r="AC87" s="62"/>
+      <c r="AD87" s="62"/>
+      <c r="AE87" s="62"/>
+      <c r="AF87" s="62"/>
+      <c r="AG87" s="62"/>
+      <c r="AH87" s="62"/>
+      <c r="AI87" s="62"/>
     </row>
     <row r="88" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B88" s="52" t="s">
@@ -26018,42 +26985,42 @@
     </row>
     <row r="66" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="67" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B67" s="61" t="s">
+      <c r="B67" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C67" s="61"/>
-      <c r="D67" s="61"/>
-      <c r="E67" s="61"/>
-      <c r="F67" s="61"/>
-      <c r="G67" s="61"/>
-      <c r="H67" s="61"/>
-      <c r="I67" s="61"/>
-      <c r="J67" s="61"/>
-      <c r="K67" s="61"/>
-      <c r="L67" s="61"/>
-      <c r="M67" s="61"/>
-      <c r="N67" s="61"/>
-      <c r="O67" s="61"/>
-      <c r="P67" s="61"/>
-      <c r="Q67" s="61"/>
-      <c r="R67" s="61"/>
-      <c r="S67" s="61"/>
-      <c r="T67" s="61"/>
-      <c r="U67" s="61"/>
-      <c r="V67" s="61"/>
-      <c r="W67" s="61"/>
-      <c r="X67" s="61"/>
-      <c r="Y67" s="61"/>
-      <c r="Z67" s="61"/>
-      <c r="AA67" s="61"/>
-      <c r="AB67" s="61"/>
-      <c r="AC67" s="61"/>
-      <c r="AD67" s="61"/>
-      <c r="AE67" s="61"/>
-      <c r="AF67" s="61"/>
-      <c r="AG67" s="61"/>
-      <c r="AH67" s="61"/>
-      <c r="AI67" s="61"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="62"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="62"/>
+      <c r="H67" s="62"/>
+      <c r="I67" s="62"/>
+      <c r="J67" s="62"/>
+      <c r="K67" s="62"/>
+      <c r="L67" s="62"/>
+      <c r="M67" s="62"/>
+      <c r="N67" s="62"/>
+      <c r="O67" s="62"/>
+      <c r="P67" s="62"/>
+      <c r="Q67" s="62"/>
+      <c r="R67" s="62"/>
+      <c r="S67" s="62"/>
+      <c r="T67" s="62"/>
+      <c r="U67" s="62"/>
+      <c r="V67" s="62"/>
+      <c r="W67" s="62"/>
+      <c r="X67" s="62"/>
+      <c r="Y67" s="62"/>
+      <c r="Z67" s="62"/>
+      <c r="AA67" s="62"/>
+      <c r="AB67" s="62"/>
+      <c r="AC67" s="62"/>
+      <c r="AD67" s="62"/>
+      <c r="AE67" s="62"/>
+      <c r="AF67" s="62"/>
+      <c r="AG67" s="62"/>
+      <c r="AH67" s="62"/>
+      <c r="AI67" s="62"/>
     </row>
     <row r="68" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B68" s="52" t="s">
@@ -49540,42 +50507,42 @@
     </row>
     <row r="274" spans="1:35" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="275" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B275" s="61" t="s">
+      <c r="B275" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="C275" s="61"/>
-      <c r="D275" s="61"/>
-      <c r="E275" s="61"/>
-      <c r="F275" s="61"/>
-      <c r="G275" s="61"/>
-      <c r="H275" s="61"/>
-      <c r="I275" s="61"/>
-      <c r="J275" s="61"/>
-      <c r="K275" s="61"/>
-      <c r="L275" s="61"/>
-      <c r="M275" s="61"/>
-      <c r="N275" s="61"/>
-      <c r="O275" s="61"/>
-      <c r="P275" s="61"/>
-      <c r="Q275" s="61"/>
-      <c r="R275" s="61"/>
-      <c r="S275" s="61"/>
-      <c r="T275" s="61"/>
-      <c r="U275" s="61"/>
-      <c r="V275" s="61"/>
-      <c r="W275" s="61"/>
-      <c r="X275" s="61"/>
-      <c r="Y275" s="61"/>
-      <c r="Z275" s="61"/>
-      <c r="AA275" s="61"/>
-      <c r="AB275" s="61"/>
-      <c r="AC275" s="61"/>
-      <c r="AD275" s="61"/>
-      <c r="AE275" s="61"/>
-      <c r="AF275" s="61"/>
-      <c r="AG275" s="61"/>
-      <c r="AH275" s="61"/>
-      <c r="AI275" s="61"/>
+      <c r="C275" s="62"/>
+      <c r="D275" s="62"/>
+      <c r="E275" s="62"/>
+      <c r="F275" s="62"/>
+      <c r="G275" s="62"/>
+      <c r="H275" s="62"/>
+      <c r="I275" s="62"/>
+      <c r="J275" s="62"/>
+      <c r="K275" s="62"/>
+      <c r="L275" s="62"/>
+      <c r="M275" s="62"/>
+      <c r="N275" s="62"/>
+      <c r="O275" s="62"/>
+      <c r="P275" s="62"/>
+      <c r="Q275" s="62"/>
+      <c r="R275" s="62"/>
+      <c r="S275" s="62"/>
+      <c r="T275" s="62"/>
+      <c r="U275" s="62"/>
+      <c r="V275" s="62"/>
+      <c r="W275" s="62"/>
+      <c r="X275" s="62"/>
+      <c r="Y275" s="62"/>
+      <c r="Z275" s="62"/>
+      <c r="AA275" s="62"/>
+      <c r="AB275" s="62"/>
+      <c r="AC275" s="62"/>
+      <c r="AD275" s="62"/>
+      <c r="AE275" s="62"/>
+      <c r="AF275" s="62"/>
+      <c r="AG275" s="62"/>
+      <c r="AH275" s="62"/>
+      <c r="AI275" s="62"/>
     </row>
     <row r="276" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B276" s="52" t="s">
@@ -50404,8 +51371,8 @@
   </sheetPr>
   <dimension ref="A1:AN93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -50488,7 +51455,7 @@
         <v>437</v>
       </c>
       <c r="O4" s="28">
-        <v>-12</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.45">
@@ -50518,7 +51485,7 @@
         <v>2019</v>
       </c>
       <c r="E7" s="56">
-        <v>2042</v>
+        <v>2050</v>
       </c>
       <c r="F7" s="56" t="s">
         <v>576</v>
@@ -50553,11 +51520,11 @@
         <v>2</v>
       </c>
       <c r="D9" s="30">
-        <f>INDEX('AEO 38'!75:75,0,MATCH(2025,'AEO 38'!1:1,0))/INDEX('AEO 38'!80:80,MATCH(2025,'AEO 38'!1:1,0))</f>
-        <v>3.9166926468788582E-2</v>
+        <f>INDEX('AEO 38'!75:75,0,MATCH(2021,'AEO 38'!1:1,0))/INDEX('AEO 38'!80:80,MATCH(2021,'AEO 38'!1:1,0))</f>
+        <v>3.0819144090348839E-2</v>
       </c>
       <c r="E9" s="16">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F9" s="9" t="str">
         <f>IF(D9=E9,"n/a",IF(OR(C9="battery electric vehicle",C9="natural gas vehicle",C9="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -50712,125 +51679,131 @@
       <c r="H10" s="31"/>
       <c r="I10" s="30">
         <f t="shared" si="0"/>
-        <v>3.9166926468788582E-2</v>
+        <v>3.0819144090348839E-2</v>
       </c>
       <c r="J10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:J$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,J$9))</f>
-        <v>5.6448671867842706E-2</v>
+        <v>4.0148104092397455E-2</v>
       </c>
       <c r="K10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:K$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,K$9))</f>
-        <v>6.4722197553938488E-2</v>
+        <v>4.4653792463561118E-2</v>
       </c>
       <c r="L10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:L$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,L$9))</f>
-        <v>7.6798648280675105E-2</v>
+        <v>5.1277042374426013E-2</v>
       </c>
       <c r="M10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:M$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,M$9))</f>
-        <v>9.4245890585342412E-2</v>
+        <v>6.0944668273484187E-2</v>
       </c>
       <c r="N10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:N$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,N$9))</f>
-        <v>0.1190820040749226</v>
+        <v>7.4911802772556088E-2</v>
       </c>
       <c r="O10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:O$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,O$9))</f>
-        <v>0.15370103640920113</v>
+        <v>9.4793989967857678E-2</v>
       </c>
       <c r="P10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:P$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,P$9))</f>
-        <v>0.20056921777729614</v>
+        <v>0.12250774967825262</v>
       </c>
       <c r="Q10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:Q$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,Q$9))</f>
-        <v>0.26157597018572998</v>
+        <v>0.16002738639012218</v>
       </c>
       <c r="R10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:R$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,R$9))</f>
-        <v>0.3370496986400533</v>
+        <v>0.20886544924044625</v>
       </c>
       <c r="S10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:S$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,S$9))</f>
-        <v>0.42476109544894347</v>
+        <v>0.26928483805044562</v>
       </c>
       <c r="T10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:T$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,T$9))</f>
-        <v>0.5195834632343943</v>
+        <v>0.33950091317215791</v>
       </c>
       <c r="U10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:U$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,U$9))</f>
-        <v>0.61440583101984514</v>
+        <v>0.41540957204517448</v>
       </c>
       <c r="V10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:V$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,V$9))</f>
-        <v>0.70211722782873531</v>
+        <v>0.49131823091819105</v>
       </c>
       <c r="W10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:W$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,W$9))</f>
-        <v>0.77759095628305863</v>
+        <v>0.56153430603990329</v>
       </c>
       <c r="X10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:X$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,X$9))</f>
-        <v>0.83859770869149242</v>
+        <v>0.62195369484990271</v>
       </c>
       <c r="Y10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:Y$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,Y$9))</f>
-        <v>0.88546589005958742</v>
+        <v>0.6707917577002267</v>
       </c>
       <c r="Z10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:Z$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,Z$9))</f>
-        <v>0.92008492239386597</v>
+        <v>0.70831139441209623</v>
       </c>
       <c r="AA10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AA$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AA$9))</f>
-        <v>0.94492103588344623</v>
+        <v>0.73602515412249125</v>
       </c>
       <c r="AB10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AB$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AB$9))</f>
-        <v>0.96236827818811355</v>
+        <v>0.7559073413177928</v>
       </c>
       <c r="AC10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AC$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AC$9))</f>
-        <v>0.97444472891485001</v>
+        <v>0.76987447581686475</v>
       </c>
       <c r="AD10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AD$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AD$9))</f>
-        <v>0.98271825460094586</v>
+        <v>0.77954210171592286</v>
       </c>
       <c r="AE10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AE$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AE$9))</f>
-        <v>0.98834659853693629</v>
+        <v>0.78616535162678769</v>
       </c>
       <c r="AF10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AF$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AF$9))</f>
-        <v>0.99215713167099218</v>
+        <v>0.79067103999795141</v>
       </c>
       <c r="AG10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AG$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AG$9))</f>
-        <v>0.99472858256613006</v>
+        <v>0.7937215065339891</v>
       </c>
       <c r="AH10" s="16">
         <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AH$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AH$9))</f>
-        <v>0.99646006045379865</v>
+        <v>0.79578004391674451</v>
       </c>
       <c r="AI10" s="16">
-        <v>1</v>
+        <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AI$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AI$9))</f>
+        <v>0.79716615320077544</v>
       </c>
       <c r="AJ10" s="16">
-        <v>1</v>
+        <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AJ$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AJ$9))</f>
+        <v>0.79809810560403771</v>
       </c>
       <c r="AK10" s="16">
-        <v>1</v>
+        <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AK$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AK$9))</f>
+        <v>0.79872408196536759</v>
       </c>
       <c r="AL10" s="16">
-        <v>1</v>
+        <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AL$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AL$9))</f>
+        <v>0.79914425858201432</v>
       </c>
       <c r="AM10" s="16">
-        <v>1</v>
+        <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AM$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AM$9))</f>
+        <v>0.79942616890305629</v>
       </c>
       <c r="AN10" s="16">
-        <v>1</v>
+        <f>IF($F9="s-curve",$D9+($E9-$D9)*$O$2/(1+EXP($O$3*(COUNT($I$9:AN$9)+$O$4))),TREND($D9:$E9,$D$7:$E$7,AN$9))</f>
+        <v>0.79961525488432961</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.45">
@@ -51575,11 +52548,11 @@
       </c>
       <c r="D16" s="30">
         <f>D9</f>
-        <v>3.9166926468788582E-2</v>
+        <v>3.0819144090348839E-2</v>
       </c>
       <c r="E16" s="16">
         <f>E9</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="F16" s="9" t="str">
         <f>IF(D16=E16,"n/a",IF(OR(C16="battery electric vehicle",C16="natural gas vehicle",C16="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -51733,131 +52706,131 @@
       <c r="H17" s="31"/>
       <c r="I17" s="30">
         <f t="shared" si="0"/>
-        <v>3.9166926468788582E-2</v>
+        <v>3.0819144090348839E-2</v>
       </c>
       <c r="J17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,J$9))</f>
-        <v>5.3362304749083656E-2</v>
+        <v>4.2183046433416922E-2</v>
       </c>
       <c r="K17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,K$9))</f>
-        <v>5.8230148407061193E-2</v>
+        <v>4.6079927436395739E-2</v>
       </c>
       <c r="L17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,L$9))</f>
-        <v>6.4722197553938501E-2</v>
+        <v>5.1277042374426027E-2</v>
       </c>
       <c r="M17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,M$9))</f>
-        <v>7.3344901586776062E-2</v>
+        <v>5.8179821900799344E-2</v>
       </c>
       <c r="N17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,N$9))</f>
-        <v>8.4735273958891508E-2</v>
+        <v>6.7298217813332228E-2</v>
       </c>
       <c r="O17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,O$9))</f>
-        <v>9.9673809719607862E-2</v>
+        <v>7.9257044001772636E-2</v>
       </c>
       <c r="P17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,P$9))</f>
-        <v>0.11908200407492263</v>
+        <v>9.4793989967857706E-2</v>
       </c>
       <c r="Q17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,Q$9))</f>
-        <v>0.14399076049065435</v>
+        <v>0.11473433039461256</v>
       </c>
       <c r="R17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,R$9))</f>
-        <v>0.17546212114079962</v>
+        <v>0.13992826760220153</v>
       </c>
       <c r="S17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,S$9))</f>
-        <v>0.21444740319819114</v>
+        <v>0.17113736463148846</v>
       </c>
       <c r="T17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,T$9))</f>
-        <v>0.26157597018573009</v>
+        <v>0.20886544924044628</v>
       </c>
       <c r="U17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,U$9))</f>
-        <v>0.31689620426733145</v>
+        <v>0.25315125306235869</v>
       </c>
       <c r="V17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,V$9))</f>
-        <v>0.37963206684425987</v>
+        <v>0.30337352975377885</v>
       </c>
       <c r="W17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,W$9))</f>
-        <v>0.44805663100484905</v>
+        <v>0.35814981324791401</v>
       </c>
       <c r="X17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,X$9))</f>
-        <v>0.5195834632343943</v>
+        <v>0.41540957204517448</v>
       </c>
       <c r="Y17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,Y$9))</f>
-        <v>0.59111029546393956</v>
+        <v>0.47266933084243495</v>
       </c>
       <c r="Z17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,Z$9))</f>
-        <v>0.65953485962452862</v>
+        <v>0.52744561433657</v>
       </c>
       <c r="AA17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AA$9))</f>
-        <v>0.72227072220145716</v>
+        <v>0.5776678910279901</v>
       </c>
       <c r="AB17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AB$9))</f>
-        <v>0.77759095628305852</v>
+        <v>0.62195369484990259</v>
       </c>
       <c r="AC17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AC$9))</f>
-        <v>0.82471952327059739</v>
+        <v>0.65968177945886042</v>
       </c>
       <c r="AD17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AD$9))</f>
-        <v>0.86370480532798899</v>
+        <v>0.6908908764881474</v>
       </c>
       <c r="AE17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AE$9))</f>
-        <v>0.89517616597813421</v>
+        <v>0.71608481369573629</v>
       </c>
       <c r="AF17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AF$9))</f>
-        <v>0.92008492239386597</v>
+        <v>0.73602515412249125</v>
       </c>
       <c r="AG17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AG$9))</f>
-        <v>0.93949311674918079</v>
+        <v>0.75156210008857627</v>
       </c>
       <c r="AH17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AH$9))</f>
-        <v>0.95443165250989714</v>
+        <v>0.76352092627701673</v>
       </c>
       <c r="AI17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AI$9))</f>
-        <v>0.96582202488201252</v>
+        <v>0.77263932218954956</v>
       </c>
       <c r="AJ17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AJ$9))</f>
-        <v>0.97444472891485001</v>
+        <v>0.77954210171592286</v>
       </c>
       <c r="AK17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AK$9))</f>
-        <v>0.98093677806172741</v>
+        <v>0.78473921665395319</v>
       </c>
       <c r="AL17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AL$9))</f>
-        <v>0.98580462171970495</v>
+        <v>0.78863609765693199</v>
       </c>
       <c r="AM17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AM$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AM$9))</f>
-        <v>0.98944338214353611</v>
+        <v>0.79154905406357012</v>
       </c>
       <c r="AN17" s="16">
         <f>IF($F16="s-curve",$D16+($E16-$D16)*$I$2/(1+EXP($I$3*(COUNT($I$9:AN$9)+$I$4))),TREND($D16:$E16,$D$8:$E$8,AN$9))</f>
-        <v>0.99215713167099218</v>
+        <v>0.7937215065339891</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.45">
@@ -52603,9 +53576,8 @@
         <f>'SYVbT-passenger'!B3/SUM('SYVbT-passenger'!3:3)</f>
         <v>3.010505804728952E-4</v>
       </c>
-      <c r="E23" s="22">
-        <f>E9</f>
-        <v>1</v>
+      <c r="E23" s="61">
+        <v>0.8</v>
       </c>
       <c r="F23" s="9" t="str">
         <f>IF(D23=E23,"n/a",IF(OR(C23="battery electric vehicle",C23="natural gas vehicle",C23="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -52764,127 +53736,127 @@
       </c>
       <c r="J24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,J$9))</f>
-        <v>1.5070634542928764E-2</v>
+        <v>1.2115828204274155E-2</v>
       </c>
       <c r="K24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,K$9))</f>
-        <v>2.01353833789924E-2</v>
+        <v>1.6167322232176901E-2</v>
       </c>
       <c r="L24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,L$9))</f>
-        <v>2.6890037116983612E-2</v>
+        <v>2.1570638401610439E-2</v>
       </c>
       <c r="M24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,M$9))</f>
-        <v>3.5861531125930435E-2</v>
+        <v>2.8747293271403202E-2</v>
       </c>
       <c r="N24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,N$9))</f>
-        <v>4.7712646171390136E-2</v>
+        <v>3.8227471535876779E-2</v>
       </c>
       <c r="O24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,O$9))</f>
-        <v>6.3255448472074108E-2</v>
+        <v>5.0660777260674819E-2</v>
       </c>
       <c r="P24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,P$9))</f>
-        <v>8.3448707885836276E-2</v>
+        <v>6.6814168587051803E-2</v>
       </c>
       <c r="Q24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,Q$9))</f>
-        <v>0.10936502811473713</v>
+        <v>8.7545663875614535E-2</v>
       </c>
       <c r="R24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,R$9))</f>
-        <v>0.14210941113553172</v>
+        <v>0.11373919815543415</v>
       </c>
       <c r="S24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,S$9))</f>
-        <v>0.18267165507699426</v>
+        <v>0.146186550315723</v>
       </c>
       <c r="T24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,T$9))</f>
-        <v>0.23170658133316255</v>
+        <v>0.18541153803296609</v>
       </c>
       <c r="U24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,U$9))</f>
-        <v>0.28926452913544826</v>
+        <v>0.23145442966044902</v>
       </c>
       <c r="V24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,V$9))</f>
-        <v>0.3545380689799798</v>
+        <v>0.2836693302251389</v>
       </c>
       <c r="W24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,W$9))</f>
-        <v>0.42573041944147549</v>
+        <v>0.34061892280380729</v>
       </c>
       <c r="X24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,X$9))</f>
-        <v>0.5001505252902364</v>
+        <v>0.40015052529023648</v>
       </c>
       <c r="Y24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,Y$9))</f>
-        <v>0.57457063113899742</v>
+        <v>0.45968212777666567</v>
       </c>
       <c r="Z24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,Z$9))</f>
-        <v>0.64576298160049306</v>
+        <v>0.516631720355334</v>
       </c>
       <c r="AA24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AA$9))</f>
-        <v>0.71103652144502461</v>
+        <v>0.56884662092002392</v>
       </c>
       <c r="AB24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AB$9))</f>
-        <v>0.76859446924731034</v>
+        <v>0.61488951254750679</v>
       </c>
       <c r="AC24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AC$9))</f>
-        <v>0.81762939550347857</v>
+        <v>0.65411450026474993</v>
       </c>
       <c r="AD24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AD$9))</f>
-        <v>0.85819163944494126</v>
+        <v>0.68656185242503887</v>
       </c>
       <c r="AE24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AE$9))</f>
-        <v>0.89093602246573578</v>
+        <v>0.71275538670485838</v>
       </c>
       <c r="AF24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AF$9))</f>
-        <v>0.91685234269463667</v>
+        <v>0.73348688199342116</v>
       </c>
       <c r="AG24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AG$9))</f>
-        <v>0.93704560210839882</v>
+        <v>0.74964027331979821</v>
       </c>
       <c r="AH24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AH$9))</f>
-        <v>0.95258840440908288</v>
+        <v>0.76207357904459627</v>
       </c>
       <c r="AI24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AI$9))</f>
-        <v>0.96443951945454254</v>
+        <v>0.77155375730906972</v>
       </c>
       <c r="AJ24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AJ$9))</f>
-        <v>0.97341101346348924</v>
+        <v>0.77873041217886241</v>
       </c>
       <c r="AK24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AK$9))</f>
-        <v>0.98016566720148057</v>
+        <v>0.78413372834829609</v>
       </c>
       <c r="AL24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AL$9))</f>
-        <v>0.98523041603754413</v>
+        <v>0.78818522237619881</v>
       </c>
       <c r="AM24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AM$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AM$9))</f>
-        <v>0.98901636499486345</v>
+        <v>0.79121375352098211</v>
       </c>
       <c r="AN24" s="16">
         <f>IF($F23="s-curve",$D23+($E23-$D23)*$I$2/(1+EXP($I$3*(COUNT($I$9:AN$9)+$I$4))),TREND($D23:$E23,$D$8:$E$8,AN$9))</f>
-        <v>0.99183988619362395</v>
+        <v>0.79347240042425593</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.45">
@@ -62926,6 +63898,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -62936,7 +63909,7 @@
   </sheetPr>
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="AH1" sqref="AH1:AI8"/>
     </sheetView>
   </sheetViews>
@@ -63085,131 +64058,131 @@
       </c>
       <c r="B2" s="16">
         <f>Data!I10</f>
-        <v>3.9166926468788582E-2</v>
+        <v>3.0819144090348839E-2</v>
       </c>
       <c r="C2" s="16">
         <f>Data!J10</f>
-        <v>5.6448671867842706E-2</v>
+        <v>4.0148104092397455E-2</v>
       </c>
       <c r="D2" s="16">
         <f>Data!K10</f>
-        <v>6.4722197553938488E-2</v>
+        <v>4.4653792463561118E-2</v>
       </c>
       <c r="E2" s="16">
         <f>Data!L10</f>
-        <v>7.6798648280675105E-2</v>
+        <v>5.1277042374426013E-2</v>
       </c>
       <c r="F2" s="16">
         <f>Data!M10</f>
-        <v>9.4245890585342412E-2</v>
+        <v>6.0944668273484187E-2</v>
       </c>
       <c r="G2" s="16">
         <f>Data!N10</f>
-        <v>0.1190820040749226</v>
+        <v>7.4911802772556088E-2</v>
       </c>
       <c r="H2" s="16">
         <f>Data!O10</f>
-        <v>0.15370103640920113</v>
+        <v>9.4793989967857678E-2</v>
       </c>
       <c r="I2" s="16">
         <f>Data!P10</f>
-        <v>0.20056921777729614</v>
+        <v>0.12250774967825262</v>
       </c>
       <c r="J2" s="16">
         <f>Data!Q10</f>
-        <v>0.26157597018572998</v>
+        <v>0.16002738639012218</v>
       </c>
       <c r="K2" s="16">
         <f>Data!R10</f>
-        <v>0.3370496986400533</v>
+        <v>0.20886544924044625</v>
       </c>
       <c r="L2" s="16">
         <f>Data!S10</f>
-        <v>0.42476109544894347</v>
+        <v>0.26928483805044562</v>
       </c>
       <c r="M2" s="16">
         <f>Data!T10</f>
-        <v>0.5195834632343943</v>
+        <v>0.33950091317215791</v>
       </c>
       <c r="N2" s="16">
         <f>Data!U10</f>
-        <v>0.61440583101984514</v>
+        <v>0.41540957204517448</v>
       </c>
       <c r="O2" s="16">
         <f>Data!V10</f>
-        <v>0.70211722782873531</v>
+        <v>0.49131823091819105</v>
       </c>
       <c r="P2" s="16">
         <f>Data!W10</f>
-        <v>0.77759095628305863</v>
+        <v>0.56153430603990329</v>
       </c>
       <c r="Q2" s="16">
         <f>Data!X10</f>
-        <v>0.83859770869149242</v>
+        <v>0.62195369484990271</v>
       </c>
       <c r="R2" s="16">
         <f>Data!Y10</f>
-        <v>0.88546589005958742</v>
+        <v>0.6707917577002267</v>
       </c>
       <c r="S2" s="16">
         <f>Data!Z10</f>
-        <v>0.92008492239386597</v>
+        <v>0.70831139441209623</v>
       </c>
       <c r="T2" s="16">
         <f>Data!AA10</f>
-        <v>0.94492103588344623</v>
+        <v>0.73602515412249125</v>
       </c>
       <c r="U2" s="16">
         <f>Data!AB10</f>
-        <v>0.96236827818811355</v>
+        <v>0.7559073413177928</v>
       </c>
       <c r="V2" s="16">
         <f>Data!AC10</f>
-        <v>0.97444472891485001</v>
+        <v>0.76987447581686475</v>
       </c>
       <c r="W2" s="16">
         <f>Data!AD10</f>
-        <v>0.98271825460094586</v>
+        <v>0.77954210171592286</v>
       </c>
       <c r="X2" s="16">
         <f>Data!AE10</f>
-        <v>0.98834659853693629</v>
+        <v>0.78616535162678769</v>
       </c>
       <c r="Y2" s="16">
         <f>Data!AF10</f>
-        <v>0.99215713167099218</v>
+        <v>0.79067103999795141</v>
       </c>
       <c r="Z2" s="16">
         <f>Data!AG10</f>
-        <v>0.99472858256613006</v>
+        <v>0.7937215065339891</v>
       </c>
       <c r="AA2" s="16">
         <f>Data!AH10</f>
-        <v>0.99646006045379865</v>
+        <v>0.79578004391674451</v>
       </c>
       <c r="AB2" s="16">
         <f>Data!AI10</f>
-        <v>1</v>
+        <v>0.79716615320077544</v>
       </c>
       <c r="AC2" s="16">
         <f>Data!AJ10</f>
-        <v>1</v>
+        <v>0.79809810560403771</v>
       </c>
       <c r="AD2" s="16">
         <f>Data!AK10</f>
-        <v>1</v>
+        <v>0.79872408196536759</v>
       </c>
       <c r="AE2" s="16">
         <f>Data!AL10</f>
-        <v>1</v>
+        <v>0.79914425858201432</v>
       </c>
       <c r="AF2" s="16">
         <f>Data!AM10</f>
-        <v>1</v>
+        <v>0.79942616890305629</v>
       </c>
       <c r="AG2" s="16">
         <f>Data!AN10</f>
-        <v>1</v>
+        <v>0.79961525488432961</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Add gasoline HDVs to freight LDV category
</commit_message>
<xml_diff>
--- a/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
+++ b/InputData/trans/MPNVbT/Max Perc New Veh by Technology.xlsx
@@ -33,7 +33,7 @@
     <sheet name="MPNVbT-motorbikes-psgr" sheetId="17" r:id="rId19"/>
     <sheet name="MPNVbT-motorbikes-frgt" sheetId="18" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -4558,131 +4558,131 @@
       </c>
       <c r="B5" s="16">
         <f>Data!I20</f>
-        <v>0.34388074989867007</v>
+        <v>0</v>
       </c>
       <c r="C5" s="16">
         <f>Data!J20</f>
-        <v>0.36504588699871476</v>
+        <v>0</v>
       </c>
       <c r="D5" s="16">
         <f>Data!K20</f>
-        <v>0.38621102409875618</v>
+        <v>0</v>
       </c>
       <c r="E5" s="16">
         <f>Data!L20</f>
-        <v>0.40737616119880471</v>
+        <v>0</v>
       </c>
       <c r="F5" s="16">
         <f>Data!M20</f>
-        <v>0.42854129829884613</v>
+        <v>0</v>
       </c>
       <c r="G5" s="16">
         <f>Data!N20</f>
-        <v>0.44970643539888755</v>
+        <v>0</v>
       </c>
       <c r="H5" s="16">
         <f>Data!O20</f>
-        <v>0.47087157249892897</v>
+        <v>0</v>
       </c>
       <c r="I5" s="16">
         <f>Data!P20</f>
-        <v>0.49203670959897039</v>
+        <v>0</v>
       </c>
       <c r="J5" s="16">
         <f>Data!Q20</f>
-        <v>0.51320184669901892</v>
+        <v>0</v>
       </c>
       <c r="K5" s="16">
         <f>Data!R20</f>
-        <v>0.53436698379906034</v>
+        <v>0</v>
       </c>
       <c r="L5" s="16">
         <f>Data!S20</f>
-        <v>0.55553212089910176</v>
+        <v>0</v>
       </c>
       <c r="M5" s="16">
         <f>Data!T20</f>
-        <v>0.57669725799914318</v>
+        <v>0</v>
       </c>
       <c r="N5" s="16">
         <f>Data!U20</f>
-        <v>0.5978623950991846</v>
+        <v>0</v>
       </c>
       <c r="O5" s="16">
         <f>Data!V20</f>
-        <v>0.61902753219923312</v>
+        <v>0</v>
       </c>
       <c r="P5" s="16">
         <f>Data!W20</f>
-        <v>0.64019266929927454</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="16">
         <f>Data!X20</f>
-        <v>0.66135780639931596</v>
+        <v>0</v>
       </c>
       <c r="R5" s="16">
         <f>Data!Y20</f>
-        <v>0.68252294349935738</v>
+        <v>0</v>
       </c>
       <c r="S5" s="16">
         <f>Data!Z20</f>
-        <v>0.70368808059940591</v>
+        <v>0</v>
       </c>
       <c r="T5" s="16">
         <f>Data!AA20</f>
-        <v>0.72485321769944733</v>
+        <v>0</v>
       </c>
       <c r="U5" s="16">
         <f>Data!AB20</f>
-        <v>0.74601835479948875</v>
+        <v>0</v>
       </c>
       <c r="V5" s="16">
         <f>Data!AC20</f>
-        <v>0.76718349189953017</v>
+        <v>0</v>
       </c>
       <c r="W5" s="16">
         <f>Data!AD20</f>
-        <v>0.78834862899957159</v>
+        <v>0</v>
       </c>
       <c r="X5" s="16">
         <f>Data!AE20</f>
-        <v>0.80951376609962011</v>
+        <v>0</v>
       </c>
       <c r="Y5" s="16">
         <f>Data!AF20</f>
-        <v>0.83067890319966153</v>
+        <v>0</v>
       </c>
       <c r="Z5" s="16">
         <f>Data!AG20</f>
-        <v>0.85184404029970295</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="16">
         <f>Data!AH20</f>
-        <v>0.87300917739974437</v>
+        <v>0</v>
       </c>
       <c r="AB5" s="16">
         <f>Data!AI20</f>
-        <v>0.89417431449978579</v>
+        <v>0</v>
       </c>
       <c r="AC5" s="16">
         <f>Data!AJ20</f>
-        <v>0.91533945159983432</v>
+        <v>0</v>
       </c>
       <c r="AD5" s="16">
         <f>Data!AK20</f>
-        <v>0.93650458869987574</v>
+        <v>0</v>
       </c>
       <c r="AE5" s="16">
         <f>Data!AL20</f>
-        <v>0.95766972579991716</v>
+        <v>0</v>
       </c>
       <c r="AF5" s="16">
         <f>Data!AM20</f>
-        <v>0.97883486289995858</v>
+        <v>0</v>
       </c>
       <c r="AG5" s="16">
         <f>Data!AN20</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.45">
@@ -5515,127 +5515,127 @@
       </c>
       <c r="C4" s="16">
         <f>Data!J26</f>
-        <v>0.10272014714675315</v>
+        <v>9.5831895834069591E-2</v>
       </c>
       <c r="D4" s="16">
         <f>Data!K26</f>
-        <v>0.10641400193163442</v>
+        <v>9.2637499306267301E-2</v>
       </c>
       <c r="E4" s="16">
         <f>Data!L26</f>
-        <v>0.1101078567165148</v>
+        <v>8.9443102778465011E-2</v>
       </c>
       <c r="F4" s="16">
         <f>Data!M26</f>
-        <v>0.11380171150139606</v>
+        <v>8.6248706250662721E-2</v>
       </c>
       <c r="G4" s="16">
         <f>Data!N26</f>
-        <v>0.11749556628627733</v>
+        <v>8.3054309722860431E-2</v>
       </c>
       <c r="H4" s="16">
         <f>Data!O26</f>
-        <v>0.1211894210711586</v>
+        <v>7.9859913195058141E-2</v>
       </c>
       <c r="I4" s="16">
         <f>Data!P26</f>
-        <v>0.12488327585603898</v>
+        <v>7.6665516667255851E-2</v>
       </c>
       <c r="J4" s="16">
         <f>Data!Q26</f>
-        <v>0.12857713064092025</v>
+        <v>7.3471120139453561E-2</v>
       </c>
       <c r="K4" s="16">
         <f>Data!R26</f>
-        <v>0.13227098542580151</v>
+        <v>7.0276723611651271E-2</v>
       </c>
       <c r="L4" s="16">
         <f>Data!S26</f>
-        <v>0.13596484021068189</v>
+        <v>6.708232708384898E-2</v>
       </c>
       <c r="M4" s="16">
         <f>Data!T26</f>
-        <v>0.13965869499556316</v>
+        <v>6.388793055604669E-2</v>
       </c>
       <c r="N4" s="16">
         <f>Data!U26</f>
-        <v>0.14335254978044443</v>
+        <v>6.06935340282444E-2</v>
       </c>
       <c r="O4" s="16">
         <f>Data!V26</f>
-        <v>0.14704640456532569</v>
+        <v>5.749913750044211E-2</v>
       </c>
       <c r="P4" s="16">
         <f>Data!W26</f>
-        <v>0.15074025935020607</v>
+        <v>5.430474097263982E-2</v>
       </c>
       <c r="Q4" s="16">
         <f>Data!X26</f>
-        <v>0.15443411413508734</v>
+        <v>5.111034444483753E-2</v>
       </c>
       <c r="R4" s="16">
         <f>Data!Y26</f>
-        <v>0.15812796891996861</v>
+        <v>4.7915947917034352E-2</v>
       </c>
       <c r="S4" s="16">
         <f>Data!Z26</f>
-        <v>0.16182182370484899</v>
+        <v>4.4721551389232062E-2</v>
       </c>
       <c r="T4" s="16">
         <f>Data!AA26</f>
-        <v>0.16551567848973026</v>
+        <v>4.1527154861429771E-2</v>
       </c>
       <c r="U4" s="16">
         <f>Data!AB26</f>
-        <v>0.16920953327461152</v>
+        <v>3.8332758333627481E-2</v>
       </c>
       <c r="V4" s="16">
         <f>Data!AC26</f>
-        <v>0.17290338805949279</v>
+        <v>3.5138361805825191E-2</v>
       </c>
       <c r="W4" s="16">
         <f>Data!AD26</f>
-        <v>0.17659724284437317</v>
+        <v>3.1943965278022901E-2</v>
       </c>
       <c r="X4" s="16">
         <f>Data!AE26</f>
-        <v>0.18029109762925444</v>
+        <v>2.8749568750220611E-2</v>
       </c>
       <c r="Y4" s="16">
         <f>Data!AF26</f>
-        <v>0.18398495241413571</v>
+        <v>2.5555172222418321E-2</v>
       </c>
       <c r="Z4" s="16">
         <f>Data!AG26</f>
-        <v>0.18767880719901608</v>
+        <v>2.2360775694616031E-2</v>
       </c>
       <c r="AA4" s="16">
         <f>Data!AH26</f>
-        <v>0.19137266198389735</v>
+        <v>1.9166379166813741E-2</v>
       </c>
       <c r="AB4" s="16">
         <f>Data!AI26</f>
-        <v>0.19506651676877862</v>
+        <v>1.5971982639011451E-2</v>
       </c>
       <c r="AC4" s="16">
         <f>Data!AJ26</f>
-        <v>0.19876037155365989</v>
+        <v>1.277758611120916E-2</v>
       </c>
       <c r="AD4" s="16">
         <f>Data!AK26</f>
-        <v>0.20245422633854027</v>
+        <v>9.5831895834068703E-3</v>
       </c>
       <c r="AE4" s="16">
         <f>Data!AL26</f>
-        <v>0.20614808112342153</v>
+        <v>6.3887930556045802E-3</v>
       </c>
       <c r="AF4" s="16">
         <f>Data!AM26</f>
-        <v>0.2098419359083028</v>
+        <v>3.1943965278022901E-3</v>
       </c>
       <c r="AG4" s="16">
         <f>Data!AN26</f>
-        <v>0.21353579069318318</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.45">
@@ -6597,131 +6597,131 @@
       </c>
       <c r="B4" s="16">
         <f>Data!I33</f>
-        <v>0.16274512438254443</v>
+        <v>0</v>
       </c>
       <c r="C4" s="16">
         <f>Data!J33</f>
-        <v>0.16438353297320996</v>
+        <v>0</v>
       </c>
       <c r="D4" s="16">
         <f>Data!K33</f>
-        <v>0.16602194156387551</v>
+        <v>0</v>
       </c>
       <c r="E4" s="16">
         <f>Data!L33</f>
-        <v>0.1676603501545415</v>
+        <v>0</v>
       </c>
       <c r="F4" s="16">
         <f>Data!M33</f>
-        <v>0.16929875874520706</v>
+        <v>0</v>
       </c>
       <c r="G4" s="16">
         <f>Data!N33</f>
-        <v>0.17093716733587305</v>
+        <v>0</v>
       </c>
       <c r="H4" s="16">
         <f>Data!O33</f>
-        <v>0.1725755759265386</v>
+        <v>0</v>
       </c>
       <c r="I4" s="16">
         <f>Data!P33</f>
-        <v>0.1742139845172046</v>
+        <v>0</v>
       </c>
       <c r="J4" s="16">
         <f>Data!Q33</f>
-        <v>0.17585239310787015</v>
+        <v>0</v>
       </c>
       <c r="K4" s="16">
         <f>Data!R33</f>
-        <v>0.17749080169853615</v>
+        <v>0</v>
       </c>
       <c r="L4" s="16">
         <f>Data!S33</f>
-        <v>0.1791292102892017</v>
+        <v>0</v>
       </c>
       <c r="M4" s="16">
         <f>Data!T33</f>
-        <v>0.1807676188798677</v>
+        <v>0</v>
       </c>
       <c r="N4" s="16">
         <f>Data!U33</f>
-        <v>0.18240602747053325</v>
+        <v>0</v>
       </c>
       <c r="O4" s="16">
         <f>Data!V33</f>
-        <v>0.18404443606119925</v>
+        <v>0</v>
       </c>
       <c r="P4" s="16">
         <f>Data!W33</f>
-        <v>0.1856828446518648</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="16">
         <f>Data!X33</f>
-        <v>0.18732125324253079</v>
+        <v>0</v>
       </c>
       <c r="R4" s="16">
         <f>Data!Y33</f>
-        <v>0.18895966183319635</v>
+        <v>0</v>
       </c>
       <c r="S4" s="16">
         <f>Data!Z33</f>
-        <v>0.19059807042386234</v>
+        <v>0</v>
       </c>
       <c r="T4" s="16">
         <f>Data!AA33</f>
-        <v>0.19223647901452789</v>
+        <v>0</v>
       </c>
       <c r="U4" s="16">
         <f>Data!AB33</f>
-        <v>0.19387488760519389</v>
+        <v>0</v>
       </c>
       <c r="V4" s="16">
         <f>Data!AC33</f>
-        <v>0.19551329619585944</v>
+        <v>0</v>
       </c>
       <c r="W4" s="16">
         <f>Data!AD33</f>
-        <v>0.19715170478652544</v>
+        <v>0</v>
       </c>
       <c r="X4" s="16">
         <f>Data!AE33</f>
-        <v>0.19879011337719099</v>
+        <v>0</v>
       </c>
       <c r="Y4" s="16">
         <f>Data!AF33</f>
-        <v>0.20042852196785699</v>
+        <v>0</v>
       </c>
       <c r="Z4" s="16">
         <f>Data!AG33</f>
-        <v>0.20206693055852254</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="16">
         <f>Data!AH33</f>
-        <v>0.20370533914918854</v>
+        <v>0</v>
       </c>
       <c r="AB4" s="16">
         <f>Data!AI33</f>
-        <v>0.20534374773985409</v>
+        <v>0</v>
       </c>
       <c r="AC4" s="16">
         <f>Data!AJ33</f>
-        <v>0.20698215633052008</v>
+        <v>0</v>
       </c>
       <c r="AD4" s="16">
         <f>Data!AK33</f>
-        <v>0.20862056492118564</v>
+        <v>0</v>
       </c>
       <c r="AE4" s="16">
         <f>Data!AL33</f>
-        <v>0.21025897351185163</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="16">
         <f>Data!AM33</f>
-        <v>0.21189738210251763</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="16">
         <f>Data!AN33</f>
-        <v>0.21353579069318318</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.45">
@@ -51372,7 +51372,7 @@
   <dimension ref="A1:AN93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -52982,15 +52982,14 @@
         <v>5</v>
       </c>
       <c r="D19" s="30">
-        <f>'SYVbT-freight'!E2/SUM('SYVbT-freight'!2:2)</f>
-        <v>0.34388074989867007</v>
+        <v>0</v>
       </c>
       <c r="E19" s="22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" s="9" t="str">
         <f>IF(D19=E19,"n/a",IF(OR(C19="battery electric vehicle",C19="natural gas vehicle",C19="plugin hybrid vehicle"),"s-curve","linear"))</f>
-        <v>linear</v>
+        <v>n/a</v>
       </c>
       <c r="H19" s="31"/>
       <c r="I19" s="30">
@@ -53141,131 +53140,131 @@
       <c r="H20" s="31"/>
       <c r="I20" s="30">
         <f t="shared" si="0"/>
-        <v>0.34388074989867007</v>
+        <v>0</v>
       </c>
       <c r="J20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,J$9))</f>
-        <v>0.36504588699871476</v>
+        <v>0</v>
       </c>
       <c r="K20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,K$9))</f>
-        <v>0.38621102409875618</v>
+        <v>0</v>
       </c>
       <c r="L20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,L$9))</f>
-        <v>0.40737616119880471</v>
+        <v>0</v>
       </c>
       <c r="M20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,M$9))</f>
-        <v>0.42854129829884613</v>
+        <v>0</v>
       </c>
       <c r="N20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,N$9))</f>
-        <v>0.44970643539888755</v>
+        <v>0</v>
       </c>
       <c r="O20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,O$9))</f>
-        <v>0.47087157249892897</v>
+        <v>0</v>
       </c>
       <c r="P20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,P$9))</f>
-        <v>0.49203670959897039</v>
+        <v>0</v>
       </c>
       <c r="Q20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,Q$9))</f>
-        <v>0.51320184669901892</v>
+        <v>0</v>
       </c>
       <c r="R20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,R$9))</f>
-        <v>0.53436698379906034</v>
+        <v>0</v>
       </c>
       <c r="S20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,S$9))</f>
-        <v>0.55553212089910176</v>
+        <v>0</v>
       </c>
       <c r="T20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,T$9))</f>
-        <v>0.57669725799914318</v>
+        <v>0</v>
       </c>
       <c r="U20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,U$9))</f>
-        <v>0.5978623950991846</v>
+        <v>0</v>
       </c>
       <c r="V20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,V$9))</f>
-        <v>0.61902753219923312</v>
+        <v>0</v>
       </c>
       <c r="W20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,W$9))</f>
-        <v>0.64019266929927454</v>
+        <v>0</v>
       </c>
       <c r="X20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,X$9))</f>
-        <v>0.66135780639931596</v>
+        <v>0</v>
       </c>
       <c r="Y20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,Y$9))</f>
-        <v>0.68252294349935738</v>
+        <v>0</v>
       </c>
       <c r="Z20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,Z$9))</f>
-        <v>0.70368808059940591</v>
+        <v>0</v>
       </c>
       <c r="AA20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AA$9))</f>
-        <v>0.72485321769944733</v>
+        <v>0</v>
       </c>
       <c r="AB20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AB$9))</f>
-        <v>0.74601835479948875</v>
+        <v>0</v>
       </c>
       <c r="AC20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AC$9))</f>
-        <v>0.76718349189953017</v>
+        <v>0</v>
       </c>
       <c r="AD20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AD$9))</f>
-        <v>0.78834862899957159</v>
+        <v>0</v>
       </c>
       <c r="AE20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AE$9))</f>
-        <v>0.80951376609962011</v>
+        <v>0</v>
       </c>
       <c r="AF20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AF$9))</f>
-        <v>0.83067890319966153</v>
+        <v>0</v>
       </c>
       <c r="AG20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AG$9))</f>
-        <v>0.85184404029970295</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AH$9))</f>
-        <v>0.87300917739974437</v>
+        <v>0</v>
       </c>
       <c r="AI20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AI$9))</f>
-        <v>0.89417431449978579</v>
+        <v>0</v>
       </c>
       <c r="AJ20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AJ$9))</f>
-        <v>0.91533945159983432</v>
+        <v>0</v>
       </c>
       <c r="AK20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AK$9))</f>
-        <v>0.93650458869987574</v>
+        <v>0</v>
       </c>
       <c r="AL20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AL$9))</f>
-        <v>0.95766972579991716</v>
+        <v>0</v>
       </c>
       <c r="AM20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AM$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AM$9))</f>
-        <v>0.97883486289995858</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="16">
         <f>IF($F19="s-curve",$D19+($E19-$D19)*$I$2/(1+EXP($I$3*(COUNT($I$9:AN$9)+$I$4))),TREND($D19:$E19,$D$8:$E$8,AN$9))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.45">
@@ -53869,7 +53868,7 @@
       </c>
       <c r="E25" s="30">
         <f>E32</f>
-        <v>0.21353579069318354</v>
+        <v>0</v>
       </c>
       <c r="F25" s="9" t="str">
         <f>IF(D25=E25,"n/a",IF(OR(C25="battery electric vehicle",C25="natural gas vehicle",C25="plugin hybrid vehicle"),"s-curve","linear"))</f>
@@ -54026,127 +54025,127 @@
       </c>
       <c r="J26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,J$9))</f>
-        <v>0.10272014714675315</v>
+        <v>9.5831895834069591E-2</v>
       </c>
       <c r="K26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,K$9))</f>
-        <v>0.10641400193163442</v>
+        <v>9.2637499306267301E-2</v>
       </c>
       <c r="L26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,L$9))</f>
-        <v>0.1101078567165148</v>
+        <v>8.9443102778465011E-2</v>
       </c>
       <c r="M26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,M$9))</f>
-        <v>0.11380171150139606</v>
+        <v>8.6248706250662721E-2</v>
       </c>
       <c r="N26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,N$9))</f>
-        <v>0.11749556628627733</v>
+        <v>8.3054309722860431E-2</v>
       </c>
       <c r="O26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,O$9))</f>
-        <v>0.1211894210711586</v>
+        <v>7.9859913195058141E-2</v>
       </c>
       <c r="P26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,P$9))</f>
-        <v>0.12488327585603898</v>
+        <v>7.6665516667255851E-2</v>
       </c>
       <c r="Q26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,Q$9))</f>
-        <v>0.12857713064092025</v>
+        <v>7.3471120139453561E-2</v>
       </c>
       <c r="R26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,R$9))</f>
-        <v>0.13227098542580151</v>
+        <v>7.0276723611651271E-2</v>
       </c>
       <c r="S26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,S$9))</f>
-        <v>0.13596484021068189</v>
+        <v>6.708232708384898E-2</v>
       </c>
       <c r="T26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,T$9))</f>
-        <v>0.13965869499556316</v>
+        <v>6.388793055604669E-2</v>
       </c>
       <c r="U26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,U$9))</f>
-        <v>0.14335254978044443</v>
+        <v>6.06935340282444E-2</v>
       </c>
       <c r="V26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,V$9))</f>
-        <v>0.14704640456532569</v>
+        <v>5.749913750044211E-2</v>
       </c>
       <c r="W26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,W$9))</f>
-        <v>0.15074025935020607</v>
+        <v>5.430474097263982E-2</v>
       </c>
       <c r="X26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,X$9))</f>
-        <v>0.15443411413508734</v>
+        <v>5.111034444483753E-2</v>
       </c>
       <c r="Y26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,Y$9))</f>
-        <v>0.15812796891996861</v>
+        <v>4.7915947917034352E-2</v>
       </c>
       <c r="Z26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,Z$9))</f>
-        <v>0.16182182370484899</v>
+        <v>4.4721551389232062E-2</v>
       </c>
       <c r="AA26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AA$9))</f>
-        <v>0.16551567848973026</v>
+        <v>4.1527154861429771E-2</v>
       </c>
       <c r="AB26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AB$9))</f>
-        <v>0.16920953327461152</v>
+        <v>3.8332758333627481E-2</v>
       </c>
       <c r="AC26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AC$9))</f>
-        <v>0.17290338805949279</v>
+        <v>3.5138361805825191E-2</v>
       </c>
       <c r="AD26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AD$9))</f>
-        <v>0.17659724284437317</v>
+        <v>3.1943965278022901E-2</v>
       </c>
       <c r="AE26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AE$9))</f>
-        <v>0.18029109762925444</v>
+        <v>2.8749568750220611E-2</v>
       </c>
       <c r="AF26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AF$9))</f>
-        <v>0.18398495241413571</v>
+        <v>2.5555172222418321E-2</v>
       </c>
       <c r="AG26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AG$9))</f>
-        <v>0.18767880719901608</v>
+        <v>2.2360775694616031E-2</v>
       </c>
       <c r="AH26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AH$9))</f>
-        <v>0.19137266198389735</v>
+        <v>1.9166379166813741E-2</v>
       </c>
       <c r="AI26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AI$9))</f>
-        <v>0.19506651676877862</v>
+        <v>1.5971982639011451E-2</v>
       </c>
       <c r="AJ26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AJ$9))</f>
-        <v>0.19876037155365989</v>
+        <v>1.277758611120916E-2</v>
       </c>
       <c r="AK26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AK$9))</f>
-        <v>0.20245422633854027</v>
+        <v>9.5831895834068703E-3</v>
       </c>
       <c r="AL26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AL$9))</f>
-        <v>0.20614808112342153</v>
+        <v>6.3887930556045802E-3</v>
       </c>
       <c r="AM26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AM$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AM$9))</f>
-        <v>0.2098419359083028</v>
+        <v>3.1943965278022901E-3</v>
       </c>
       <c r="AN26" s="16">
         <f>IF($F25="s-curve",$D25+($E25-$D25)*$I$2/(1+EXP($I$3*(COUNT($I$9:AN$9)+$I$4))),TREND($D25:$E25,$D$8:$E$8,AN$9))</f>
-        <v>0.21353579069318318</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.45">
@@ -54892,16 +54891,14 @@
         <v>4</v>
       </c>
       <c r="D32" s="30">
-        <f>SUM(INDEX('AEO 49'!$212:$212,MATCH(D$8,'AEO 49'!$1:$1,0)),INDEX('AEO 49'!$223:$223,MATCH(D$8,'AEO 49'!$1:$1,0)),INDEX('AEO 49'!$234:$234,MATCH(D$8,'AEO 49'!$1:$1,0)))/INDEX('AEO 49'!$243:$243,MATCH(D$8,'AEO 49'!$1:$1,0))</f>
-        <v>0.16274512438254443</v>
+        <v>0</v>
       </c>
       <c r="E32" s="30">
-        <f>SUM(INDEX('AEO 49'!$212:$212,MATCH(E$8,'AEO 49'!$1:$1,0)),INDEX('AEO 49'!$223:$223,MATCH(E$8,'AEO 49'!$1:$1,0)),INDEX('AEO 49'!$234:$234,MATCH(E$8,'AEO 49'!$1:$1,0)))/INDEX('AEO 49'!$243:$243,MATCH(E$8,'AEO 49'!$1:$1,0))</f>
-        <v>0.21353579069318354</v>
+        <v>0</v>
       </c>
       <c r="F32" s="9" t="str">
         <f>IF(D32=E32,"n/a",IF(OR(C32="battery electric vehicle",C32="natural gas vehicle",C32="plugin hybrid vehicle"),"s-curve","linear"))</f>
-        <v>linear</v>
+        <v>n/a</v>
       </c>
       <c r="H32" s="31"/>
       <c r="I32" s="30">
@@ -55050,131 +55047,131 @@
       <c r="H33" s="31"/>
       <c r="I33" s="30">
         <f t="shared" si="0"/>
-        <v>0.16274512438254443</v>
+        <v>0</v>
       </c>
       <c r="J33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:J$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,J$9))</f>
-        <v>0.16438353297320996</v>
+        <v>0</v>
       </c>
       <c r="K33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:K$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,K$9))</f>
-        <v>0.16602194156387551</v>
+        <v>0</v>
       </c>
       <c r="L33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:L$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,L$9))</f>
-        <v>0.1676603501545415</v>
+        <v>0</v>
       </c>
       <c r="M33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:M$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,M$9))</f>
-        <v>0.16929875874520706</v>
+        <v>0</v>
       </c>
       <c r="N33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:N$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,N$9))</f>
-        <v>0.17093716733587305</v>
+        <v>0</v>
       </c>
       <c r="O33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:O$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,O$9))</f>
-        <v>0.1725755759265386</v>
+        <v>0</v>
       </c>
       <c r="P33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:P$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,P$9))</f>
-        <v>0.1742139845172046</v>
+        <v>0</v>
       </c>
       <c r="Q33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:Q$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,Q$9))</f>
-        <v>0.17585239310787015</v>
+        <v>0</v>
       </c>
       <c r="R33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:R$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,R$9))</f>
-        <v>0.17749080169853615</v>
+        <v>0</v>
       </c>
       <c r="S33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:S$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,S$9))</f>
-        <v>0.1791292102892017</v>
+        <v>0</v>
       </c>
       <c r="T33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:T$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,T$9))</f>
-        <v>0.1807676188798677</v>
+        <v>0</v>
       </c>
       <c r="U33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:U$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,U$9))</f>
-        <v>0.18240602747053325</v>
+        <v>0</v>
       </c>
       <c r="V33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:V$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,V$9))</f>
-        <v>0.18404443606119925</v>
+        <v>0</v>
       </c>
       <c r="W33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:W$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,W$9))</f>
-        <v>0.1856828446518648</v>
+        <v>0</v>
       </c>
       <c r="X33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:X$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,X$9))</f>
-        <v>0.18732125324253079</v>
+        <v>0</v>
       </c>
       <c r="Y33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:Y$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,Y$9))</f>
-        <v>0.18895966183319635</v>
+        <v>0</v>
       </c>
       <c r="Z33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:Z$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,Z$9))</f>
-        <v>0.19059807042386234</v>
+        <v>0</v>
       </c>
       <c r="AA33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AA$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AA$9))</f>
-        <v>0.19223647901452789</v>
+        <v>0</v>
       </c>
       <c r="AB33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AB$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AB$9))</f>
-        <v>0.19387488760519389</v>
+        <v>0</v>
       </c>
       <c r="AC33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AC$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AC$9))</f>
-        <v>0.19551329619585944</v>
+        <v>0</v>
       </c>
       <c r="AD33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AD$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AD$9))</f>
-        <v>0.19715170478652544</v>
+        <v>0</v>
       </c>
       <c r="AE33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AE$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AE$9))</f>
-        <v>0.19879011337719099</v>
+        <v>0</v>
       </c>
       <c r="AF33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AF$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AF$9))</f>
-        <v>0.20042852196785699</v>
+        <v>0</v>
       </c>
       <c r="AG33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AG$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AG$9))</f>
-        <v>0.20206693055852254</v>
+        <v>0</v>
       </c>
       <c r="AH33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AH$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AH$9))</f>
-        <v>0.20370533914918854</v>
+        <v>0</v>
       </c>
       <c r="AI33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AI$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AI$9))</f>
-        <v>0.20534374773985409</v>
+        <v>0</v>
       </c>
       <c r="AJ33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AJ$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AJ$9))</f>
-        <v>0.20698215633052008</v>
+        <v>0</v>
       </c>
       <c r="AK33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AK$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AK$9))</f>
-        <v>0.20862056492118564</v>
+        <v>0</v>
       </c>
       <c r="AL33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AL$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AL$9))</f>
-        <v>0.21025897351185163</v>
+        <v>0</v>
       </c>
       <c r="AM33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AM$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AM$9))</f>
-        <v>0.21189738210251763</v>
+        <v>0</v>
       </c>
       <c r="AN33" s="16">
         <f>IF($F32="s-curve",$D32+($E32-$D32)*$I$2/(1+EXP($I$3*(COUNT($I$9:AN$9)+$I$4))),TREND($D32:$E32,$D$8:$E$8,AN$9))</f>
-        <v>0.21353579069318318</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.45">

</xml_diff>